<commit_message>
Actualiza pipeline y configuraciones
</commit_message>
<xml_diff>
--- a/data/input/matriz_servicios_consolidada.xlsx
+++ b/data/input/matriz_servicios_consolidada.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Desktop\Escritorio_archivos\Proyecto_alcaldia\Entregable_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Desktop\Escritorio_archivos\Proyecto_alcaldia\Entregable_4\gobierno-datos-cali\catalogo_servicios_alcaldia_cali\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443B160A-A08B-4904-8075-3FFE3D7BEF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C2A149-D709-424F-8FE4-637D433193E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5E867AA7-73AA-458A-9098-63D488401122}"/>
   </bookViews>
@@ -1301,11 +1301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8FD959D-5731-41CD-A9CB-B44DE7069ED4}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:R55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,7 +1384,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1441,7 +1440,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1497,7 +1496,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3065,7 +3064,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="300" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>1</v>
       </c>
@@ -3121,7 +3120,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>2</v>
       </c>
@@ -3177,7 +3176,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>3</v>
       </c>
@@ -3233,7 +3232,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>4</v>
       </c>
@@ -3289,7 +3288,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>5</v>
       </c>
@@ -3345,7 +3344,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>6</v>
       </c>
@@ -3401,7 +3400,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>7</v>
       </c>
@@ -3457,7 +3456,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>8</v>
       </c>
@@ -3513,7 +3512,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>9</v>
       </c>
@@ -3569,7 +3568,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>10</v>
       </c>
@@ -3625,7 +3624,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>11</v>
       </c>
@@ -3681,7 +3680,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>12</v>
       </c>
@@ -3737,7 +3736,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>13</v>
       </c>
@@ -3793,7 +3792,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>14</v>
       </c>
@@ -3905,7 +3904,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>2</v>
       </c>
@@ -3961,7 +3960,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="270" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="270" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>3</v>
       </c>
@@ -4017,7 +4016,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>4</v>
       </c>
@@ -4073,7 +4072,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>5</v>
       </c>
@@ -4129,7 +4128,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>6</v>
       </c>
@@ -4185,7 +4184,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" ht="135" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>7</v>
       </c>
@@ -4241,7 +4240,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="53" spans="1:18" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" ht="150" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>8</v>
       </c>
@@ -4297,7 +4296,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" ht="135" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>9</v>
       </c>
@@ -4410,13 +4409,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R55" xr:uid="{B8FD959D-5731-41CD-A9CB-B44DE7069ED4}">
-    <filterColumn colId="13">
-      <filters>
-        <filter val="99"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:R55" xr:uid="{B8FD959D-5731-41CD-A9CB-B44DE7069ED4}"/>
   <hyperlinks>
     <hyperlink ref="R45" r:id="rId1" xr:uid="{D9D65EFD-C0AA-473C-ACF9-765BCE542E3D}"/>
   </hyperlinks>

</xml_diff>